<commit_message>
add 2019 to files, update calibration
</commit_message>
<xml_diff>
--- a/InputData/ctrl-settings/EGGRA/Exogenous GDP Growth Rate Adjustment.xlsx
+++ b/InputData/ctrl-settings/EGGRA/Exogenous GDP Growth Rate Adjustment.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jeff Rissman\CodeRepositories\eps-us\InputData\ctrl-settings\EGGRA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olivia\Documents\EPS_Models by Region\Canada\canada-eps\InputData\ctrl-settings\EGGRA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02D77B80-46D1-401E-A779-175C6F49CDE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7906C134-37BF-43F4-8D66-4AEACCE21858}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9555" yWindow="345" windowWidth="22590" windowHeight="21675" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11475" yWindow="225" windowWidth="17025" windowHeight="17175" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -201,7 +201,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -211,7 +211,6 @@
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -498,7 +497,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -522,7 +521,7 @@
       <c r="A4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" t="s">
         <v>25</v>
       </c>
     </row>
@@ -664,114 +663,120 @@
   <sheetPr>
     <tabColor theme="8" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:AF2"/>
+  <dimension ref="A1:AG2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="51.140625" customWidth="1"/>
+    <col min="2" max="2" width="5.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B1">
+      <c r="B1" s="5">
+        <v>2019</v>
+      </c>
+      <c r="C1">
         <v>2020</v>
       </c>
-      <c r="C1">
+      <c r="D1">
         <v>2021</v>
       </c>
-      <c r="D1">
+      <c r="E1">
         <v>2022</v>
       </c>
-      <c r="E1">
+      <c r="F1">
         <v>2023</v>
       </c>
-      <c r="F1">
+      <c r="G1">
         <v>2024</v>
       </c>
-      <c r="G1">
+      <c r="H1">
         <v>2025</v>
       </c>
-      <c r="H1">
+      <c r="I1">
         <v>2026</v>
       </c>
-      <c r="I1">
+      <c r="J1">
         <v>2027</v>
       </c>
-      <c r="J1">
+      <c r="K1">
         <v>2028</v>
       </c>
-      <c r="K1">
+      <c r="L1">
         <v>2029</v>
       </c>
-      <c r="L1">
+      <c r="M1">
         <v>2030</v>
       </c>
-      <c r="M1">
+      <c r="N1">
         <v>2031</v>
       </c>
-      <c r="N1">
+      <c r="O1">
         <v>2032</v>
       </c>
-      <c r="O1">
+      <c r="P1">
         <v>2033</v>
       </c>
-      <c r="P1">
+      <c r="Q1">
         <v>2034</v>
       </c>
-      <c r="Q1">
+      <c r="R1">
         <v>2035</v>
       </c>
-      <c r="R1">
+      <c r="S1">
         <v>2036</v>
       </c>
-      <c r="S1">
+      <c r="T1">
         <v>2037</v>
       </c>
-      <c r="T1">
+      <c r="U1">
         <v>2038</v>
       </c>
-      <c r="U1">
+      <c r="V1">
         <v>2039</v>
       </c>
-      <c r="V1">
+      <c r="W1">
         <v>2040</v>
       </c>
-      <c r="W1">
+      <c r="X1">
         <v>2041</v>
       </c>
-      <c r="X1">
+      <c r="Y1">
         <v>2042</v>
       </c>
-      <c r="Y1">
+      <c r="Z1">
         <v>2043</v>
       </c>
-      <c r="Z1">
+      <c r="AA1">
         <v>2044</v>
       </c>
-      <c r="AA1">
+      <c r="AB1">
         <v>2045</v>
       </c>
-      <c r="AB1">
+      <c r="AC1">
         <v>2046</v>
       </c>
-      <c r="AC1">
+      <c r="AD1">
         <v>2047</v>
       </c>
-      <c r="AD1">
+      <c r="AE1">
         <v>2048</v>
       </c>
-      <c r="AE1">
+      <c r="AF1">
         <v>2049</v>
       </c>
-      <c r="AF1">
+      <c r="AG1">
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -866,6 +871,9 @@
         <v>0</v>
       </c>
       <c r="AF2">
+        <v>0</v>
+      </c>
+      <c r="AG2">
         <v>0</v>
       </c>
     </row>
@@ -882,7 +890,9 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -894,7 +904,7 @@
       <c r="A1" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="7" t="s">
         <v>30</v>
       </c>
     </row>
@@ -903,7 +913,7 @@
         <v>32</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>